<commit_message>
Forgot to add final update to BoM
</commit_message>
<xml_diff>
--- a/hardware/uob-hep-pc068a-cryosub/cryosub_power_converter_top_v03/cryosub_power_converter_top_bom_v03.xlsx
+++ b/hardware/uob-hep-pc068a-cryosub/cryosub_power_converter_top_v03/cryosub_power_converter_top_bom_v03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phdgc/Documents/DUNE/cryosub/hardware/uob-hep-pc068a-cryosub/cryosub_power_converter_top_v03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22111F86-A6C7-A84C-8C3F-A2AFC22F23E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3682E82A-6C19-E349-AFA6-287BE080A246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2860" windowWidth="27240" windowHeight="15020" xr2:uid="{7AE3736D-B4A5-1241-AD38-3A07FD10F958}"/>
+    <workbookView xWindow="420" yWindow="500" windowWidth="27240" windowHeight="15020" xr2:uid="{7AE3736D-B4A5-1241-AD38-3A07FD10F958}"/>
   </bookViews>
   <sheets>
     <sheet name="cryosub_power_converter_top_bom" sheetId="2" r:id="rId1"/>

</xml_diff>